<commit_message>
student data migration done
</commit_message>
<xml_diff>
--- a/TrainersSchoolingSystem/App_Data/uploads/Template.xlsx
+++ b/TrainersSchoolingSystem/App_Data/uploads/Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D39EDE4-61C7-4BBC-8C36-551A12CAEB8A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C0F69A-E88A-4078-97DA-65EA56054A08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Designations" sheetId="1" r:id="rId1"/>
@@ -2349,7 +2349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2564,7 +2564,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C16"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3400,8 +3400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821090AC-0EFF-46BC-8676-16B3DD222A59}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3434,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3448,7 +3448,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3476,7 +3476,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3490,7 +3490,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,7 +3504,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3518,7 +3518,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3532,7 +3532,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3560,7 +3560,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,7 +3574,7 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3588,7 +3588,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3602,7 +3602,7 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>